<commit_message>
adding Q variable for objective
</commit_message>
<xml_diff>
--- a/Documents/connections.xlsx
+++ b/Documents/connections.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericgero/Documents/MSDS_460_Final_Project/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericgero/Desktop/MSDS-460/MSDS_460_Final_Project/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{EE814FC3-6F9D-6840-A5C7-DC3C68C81ED5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{136DE8A9-B2C9-F044-B6A8-A6BEF3C8440D}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16360" xr2:uid="{C6A16760-A1C5-F347-949F-6A11DE09A74F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C6A16760-A1C5-F347-949F-6A11DE09A74F}"/>
   </bookViews>
   <sheets>
     <sheet name="Solver (2)" sheetId="5" r:id="rId1"/>
@@ -89,7 +89,7 @@
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="87">
   <si>
     <t xml:space="preserve">From </t>
   </si>
@@ -343,6 +343,30 @@
   <si>
     <t>1-3-4-6-7-9-10-12-13-15-16-18-19-21-22-23-25</t>
   </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>% Deviation</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Weighted % Deviation</t>
+  </si>
+  <si>
+    <t>Minimax Objective</t>
+  </si>
+  <si>
+    <t>var and objective</t>
+  </si>
+  <si>
+    <t>make constraints from each colum</t>
+  </si>
 </sst>
 </file>
 
@@ -398,7 +422,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,6 +486,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,12 +575,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -639,15 +670,6 @@
     <xf numFmtId="164" fontId="1" fillId="10" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="46" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -662,14 +684,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="45"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -678,9 +694,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -691,13 +704,64 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="8" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="46" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="46" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="10" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -735,26 +799,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -900,31 +944,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1240,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9337B6EB-7947-4849-B32B-8444BA3D7EC1}">
   <dimension ref="A1:W78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B73" sqref="A73:XFD73"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P56" sqref="P56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1264,54 +1288,54 @@
   <sheetData>
     <row r="1" spans="1:23" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="57"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+      <c r="O1" s="60"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="60"/>
+      <c r="R1" s="60"/>
+      <c r="S1" s="20"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54" t="s">
+      <c r="C2" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="54"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
       <c r="N2" s="20"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="54" t="s">
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="R2" s="54"/>
+      <c r="R2" s="61"/>
       <c r="S2" s="20"/>
     </row>
     <row r="3" spans="1:23" ht="32" x14ac:dyDescent="0.2">
@@ -3017,10 +3041,10 @@
         <v>0.2019230769230769</v>
       </c>
       <c r="N30" s="20"/>
-      <c r="O30" s="43" t="s">
+      <c r="O30" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="P30" s="43"/>
+      <c r="P30" s="59"/>
       <c r="Q30" s="34"/>
       <c r="R30" s="34"/>
       <c r="S30" s="20"/>
@@ -3072,10 +3096,10 @@
         <v>0.26794871794871794</v>
       </c>
       <c r="N31" s="20"/>
-      <c r="O31" s="60" t="s">
+      <c r="O31" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="P31" s="46">
+      <c r="P31" s="43">
         <f>SUMPRODUCT($B$4:$B$57,$H$4:$H$57)</f>
         <v>4487</v>
       </c>
@@ -3134,14 +3158,14 @@
         <v>6.4102564102564097</v>
       </c>
       <c r="N32" s="20"/>
-      <c r="O32" s="61" t="s">
+      <c r="O32" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="P32" s="58">
+      <c r="P32" s="52">
         <f>SUMPRODUCT($B$4:$B$57,$I$4:$I$57)/COUNTIF($B$4:$B$57, "&gt;0")</f>
         <v>41.8125</v>
       </c>
-      <c r="Q32" s="62">
+      <c r="Q32" s="56">
         <f>SUMPRODUCT($B$4:$B$57,$I$4:$I$57)</f>
         <v>669</v>
       </c>
@@ -3197,10 +3221,10 @@
         <v>0.16602564102564102</v>
       </c>
       <c r="N33" s="20"/>
-      <c r="O33" s="61" t="s">
+      <c r="O33" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="P33" s="59">
+      <c r="P33" s="53">
         <f>SUMPRODUCT($B$4:$B$57,$K$4:$K$57)</f>
         <v>3496.1499999999996</v>
       </c>
@@ -3259,10 +3283,10 @@
         <v>6.4102564102564097</v>
       </c>
       <c r="N34" s="20"/>
-      <c r="O34" s="61" t="s">
+      <c r="O34" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="P34" s="48">
+      <c r="P34" s="45">
         <f>SUMPRODUCT($B$4:$B$57,$M$4:$M$57)</f>
         <v>2.8762820512820508</v>
       </c>
@@ -3741,10 +3765,16 @@
         <v>6.4102564102564097</v>
       </c>
       <c r="N43" s="20"/>
-      <c r="O43" s="20"/>
-      <c r="P43" s="20"/>
-      <c r="Q43" s="20"/>
-      <c r="R43" s="20"/>
+      <c r="O43" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="P43" s="70"/>
+      <c r="Q43" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="R43" s="20" t="s">
+        <v>83</v>
+      </c>
       <c r="S43" s="20"/>
       <c r="W43" s="23">
         <v>25</v>
@@ -3794,10 +3824,20 @@
         <v>0.1730769230769231</v>
       </c>
       <c r="N44" s="20"/>
-      <c r="O44" s="20"/>
-      <c r="P44" s="20"/>
-      <c r="Q44" s="20"/>
-      <c r="R44" s="20"/>
+      <c r="O44" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="P44" s="71">
+        <f>(P31-O61)/O61</f>
+        <v>1.0139138240574506</v>
+      </c>
+      <c r="Q44" s="69">
+        <v>1</v>
+      </c>
+      <c r="R44" s="20">
+        <f>P44*Q44</f>
+        <v>1.0139138240574506</v>
+      </c>
       <c r="S44" s="20"/>
       <c r="W44" s="23">
         <v>37</v>
@@ -3847,10 +3887,20 @@
         <v>6.4102564102564097</v>
       </c>
       <c r="N45" s="20"/>
-      <c r="O45" s="20"/>
-      <c r="P45" s="20"/>
-      <c r="Q45" s="20"/>
-      <c r="R45" s="20"/>
+      <c r="O45" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="P45" s="71">
+        <f>(P32-P61)/P61</f>
+        <v>-5.6364251861882243E-2</v>
+      </c>
+      <c r="Q45" s="69">
+        <v>1</v>
+      </c>
+      <c r="R45" s="20">
+        <f>P45*Q45</f>
+        <v>-5.6364251861882243E-2</v>
+      </c>
       <c r="S45" s="20"/>
       <c r="W45" s="23">
         <v>31</v>
@@ -3900,10 +3950,20 @@
         <v>6.4102564102564097</v>
       </c>
       <c r="N46" s="20"/>
-      <c r="O46" s="20"/>
-      <c r="P46" s="20"/>
-      <c r="Q46" s="20"/>
-      <c r="R46" s="20"/>
+      <c r="O46" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="P46" s="71">
+        <f>(P33-Q61)/Q61</f>
+        <v>1.889690627918702</v>
+      </c>
+      <c r="Q46" s="69">
+        <v>1</v>
+      </c>
+      <c r="R46" s="20">
+        <f>P46*Q46</f>
+        <v>1.889690627918702</v>
+      </c>
       <c r="S46" s="20"/>
       <c r="W46" s="23">
         <v>30</v>
@@ -3953,10 +4013,20 @@
         <v>0.16025641025641027</v>
       </c>
       <c r="N47" s="20"/>
-      <c r="O47" s="20"/>
-      <c r="P47" s="20"/>
-      <c r="Q47" s="20"/>
-      <c r="R47" s="20"/>
+      <c r="O47" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="P47" s="71">
+        <f>(P34-R61)/R61</f>
+        <v>1.0145166117928761</v>
+      </c>
+      <c r="Q47" s="69">
+        <v>1</v>
+      </c>
+      <c r="R47" s="20">
+        <f>P47*Q47</f>
+        <v>1.0145166117928761</v>
+      </c>
       <c r="S47" s="20"/>
       <c r="W47" s="23">
         <v>36</v>
@@ -4112,7 +4182,9 @@
         <v>6.4102564102564097</v>
       </c>
       <c r="N50" s="20"/>
-      <c r="O50" s="20"/>
+      <c r="O50" s="20" t="s">
+        <v>84</v>
+      </c>
       <c r="P50" s="20"/>
       <c r="Q50" s="20"/>
       <c r="R50" s="20"/>
@@ -4165,8 +4237,10 @@
         <v>0.16025641025641027</v>
       </c>
       <c r="N51" s="20"/>
-      <c r="O51" s="20"/>
-      <c r="P51" s="33"/>
+      <c r="O51" s="64"/>
+      <c r="P51" s="33" t="s">
+        <v>85</v>
+      </c>
       <c r="Q51" s="34"/>
       <c r="R51" s="20"/>
       <c r="S51" s="20"/>
@@ -4272,7 +4346,9 @@
       </c>
       <c r="N53" s="20"/>
       <c r="O53" s="20"/>
-      <c r="P53" s="20"/>
+      <c r="P53" s="20" t="s">
+        <v>86</v>
+      </c>
       <c r="Q53" s="20"/>
       <c r="R53" s="20"/>
       <c r="S53" s="20"/>
@@ -4377,10 +4453,18 @@
         <v>0.27692307692307694</v>
       </c>
       <c r="N55" s="20"/>
-      <c r="O55" s="20"/>
-      <c r="P55" s="20"/>
-      <c r="Q55" s="20"/>
-      <c r="R55" s="20"/>
+      <c r="O55" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="P55" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q55" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="R55" s="20" t="s">
+        <v>5</v>
+      </c>
       <c r="S55" s="20"/>
       <c r="W55" s="23">
         <v>36</v>
@@ -4430,11 +4514,21 @@
         <v>0.22884615384615384</v>
       </c>
       <c r="N56" s="20"/>
-      <c r="O56" s="20"/>
-      <c r="P56" s="20"/>
-      <c r="Q56" s="20"/>
-      <c r="R56" s="20"/>
-      <c r="S56" s="20"/>
+      <c r="O56" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="P56" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q56" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="R56" s="71" t="s">
+        <v>5</v>
+      </c>
+      <c r="S56" s="20" t="s">
+        <v>5</v>
+      </c>
       <c r="W56" s="23">
         <v>40</v>
       </c>
@@ -4525,7 +4619,7 @@
       <c r="G59" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="H59" s="46">
+      <c r="H59" s="43">
         <f>SUMPRODUCT($B$4:$B$57,$H$4:$H$57)</f>
         <v>4487</v>
       </c>
@@ -4534,12 +4628,12 @@
         <v>41.8125</v>
       </c>
       <c r="J59" s="23"/>
-      <c r="K59" s="47">
+      <c r="K59" s="44">
         <f>SUMPRODUCT($B4:B$57,$K$4:$K$57)</f>
         <v>3496.1499999999996</v>
       </c>
-      <c r="L59" s="47"/>
-      <c r="M59" s="48">
+      <c r="L59" s="44"/>
+      <c r="M59" s="45">
         <f>SUMPRODUCT($B$4:$B$57,$M$4:$M$57)</f>
         <v>2.8762820512820508</v>
       </c>
@@ -4557,11 +4651,11 @@
       <c r="D60" s="20"/>
       <c r="E60" s="20"/>
       <c r="F60" s="20"/>
-      <c r="G60" s="42" t="s">
+      <c r="G60" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="H60" s="42"/>
-      <c r="I60" s="42"/>
+      <c r="H60" s="62"/>
+      <c r="I60" s="62"/>
       <c r="J60" s="38"/>
       <c r="K60" s="36" t="s">
         <v>5</v>
@@ -4571,7 +4665,9 @@
         <v>5</v>
       </c>
       <c r="N60" s="20"/>
-      <c r="O60" s="20"/>
+      <c r="O60" s="20" t="s">
+        <v>79</v>
+      </c>
       <c r="P60" s="20"/>
       <c r="Q60" s="20"/>
       <c r="R60" s="20"/>
@@ -4592,10 +4688,18 @@
       <c r="L61" s="21"/>
       <c r="M61" s="20"/>
       <c r="N61" s="20"/>
-      <c r="O61" s="20"/>
-      <c r="P61" s="20"/>
-      <c r="Q61" s="20"/>
-      <c r="R61" s="20"/>
+      <c r="O61" s="20">
+        <v>2228</v>
+      </c>
+      <c r="P61" s="20">
+        <v>44.31</v>
+      </c>
+      <c r="Q61" s="20">
+        <v>1209.8699999999999</v>
+      </c>
+      <c r="R61" s="68">
+        <v>1.4277777777777778</v>
+      </c>
       <c r="S61" s="20"/>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.2">
@@ -4635,27 +4739,27 @@
       <c r="F67" s="39" t="s">
         <v>53</v>
       </c>
-      <c r="G67" s="52" t="s">
+      <c r="G67" s="48" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="51" t="s">
+      <c r="A68" s="58" t="s">
         <v>66</v>
       </c>
       <c r="B68" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C68" s="8">
+      <c r="C68" s="65">
         <v>2797</v>
       </c>
       <c r="D68" s="8">
         <v>41.8</v>
       </c>
-      <c r="E68" s="49">
+      <c r="E68" s="46">
         <v>2011.84</v>
       </c>
-      <c r="F68" s="45">
+      <c r="F68" s="42">
         <v>1.7923611111111111</v>
       </c>
       <c r="G68" s="12" t="s">
@@ -4663,7 +4767,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="67" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="51"/>
+      <c r="A69" s="58"/>
       <c r="B69" s="8" t="s">
         <v>76</v>
       </c>
@@ -4673,10 +4777,10 @@
       <c r="D69" s="8">
         <v>41.81</v>
       </c>
-      <c r="E69" s="49">
+      <c r="E69" s="46">
         <v>3496.15</v>
       </c>
-      <c r="F69" s="45">
+      <c r="F69" s="42">
         <v>2.5006944444444446</v>
       </c>
       <c r="G69" s="12" t="s">
@@ -4684,7 +4788,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="51"/>
+      <c r="A70" s="58"/>
       <c r="B70" s="8" t="s">
         <v>54</v>
       </c>
@@ -4694,10 +4798,10 @@
       <c r="D70" s="8">
         <v>41.8</v>
       </c>
-      <c r="E70" s="49">
+      <c r="E70" s="46">
         <v>2011.84</v>
       </c>
-      <c r="F70" s="45">
+      <c r="F70" s="42">
         <v>1.83402777777778</v>
       </c>
       <c r="G70" s="12" t="s">
@@ -4705,7 +4809,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="51"/>
+      <c r="A71" s="58"/>
       <c r="B71" s="8" t="s">
         <v>53</v>
       </c>
@@ -4715,10 +4819,10 @@
       <c r="D71" s="8">
         <v>41.8</v>
       </c>
-      <c r="E71" s="49">
+      <c r="E71" s="46">
         <v>2011.84</v>
       </c>
-      <c r="F71" s="45">
+      <c r="F71" s="42">
         <v>1.8756944444444399</v>
       </c>
       <c r="G71" s="12" t="s">
@@ -4726,22 +4830,22 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="51" t="s">
+      <c r="A72" s="58" t="s">
         <v>67</v>
       </c>
       <c r="B72" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="C72" s="8">
+      <c r="C72" s="64">
         <v>2228</v>
       </c>
       <c r="D72" s="8">
         <v>40.25</v>
       </c>
-      <c r="E72" s="49">
+      <c r="E72" s="46">
         <v>1716.03</v>
       </c>
-      <c r="F72" s="45">
+      <c r="F72" s="42">
         <v>1.4277777777777778</v>
       </c>
       <c r="G72" s="12" t="s">
@@ -4749,20 +4853,20 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="62" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="51"/>
+      <c r="A73" s="58"/>
       <c r="B73" s="8" t="s">
         <v>76</v>
       </c>
       <c r="C73" s="8">
         <v>5873</v>
       </c>
-      <c r="D73" s="8">
+      <c r="D73" s="64">
         <v>44.31</v>
       </c>
-      <c r="E73" s="63">
+      <c r="E73" s="57">
         <v>4582.01</v>
       </c>
-      <c r="F73" s="45">
+      <c r="F73" s="42">
         <v>3.8062499999999999</v>
       </c>
       <c r="G73" s="12" t="s">
@@ -4770,7 +4874,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="51"/>
+      <c r="A74" s="58"/>
       <c r="B74" s="8" t="s">
         <v>54</v>
       </c>
@@ -4780,10 +4884,10 @@
       <c r="D74" s="8">
         <v>39.78</v>
       </c>
-      <c r="E74" s="49">
+      <c r="E74" s="66">
         <v>1209.8699999999999</v>
       </c>
-      <c r="F74" s="45">
+      <c r="F74" s="42">
         <v>1.55</v>
       </c>
       <c r="G74" s="12" t="s">
@@ -4791,7 +4895,7 @@
       </c>
     </row>
     <row r="75" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="51"/>
+      <c r="A75" s="58"/>
       <c r="B75" s="8" t="s">
         <v>53</v>
       </c>
@@ -4801,10 +4905,10 @@
       <c r="D75" s="8">
         <v>40.25</v>
       </c>
-      <c r="E75" s="49">
+      <c r="E75" s="46">
         <v>1716.03</v>
       </c>
-      <c r="F75" s="45">
+      <c r="F75" s="67">
         <v>1.4277777777777778</v>
       </c>
       <c r="G75" s="12" t="s">
@@ -4812,7 +4916,7 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="51" t="s">
+      <c r="A76" s="58" t="s">
         <v>72</v>
       </c>
       <c r="B76" s="8" t="s">
@@ -4824,10 +4928,10 @@
       <c r="D76" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E76" s="49" t="s">
+      <c r="E76" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="F76" s="45" t="s">
+      <c r="F76" s="42" t="s">
         <v>5</v>
       </c>
       <c r="G76" s="12" t="s">
@@ -4835,7 +4939,7 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="51"/>
+      <c r="A77" s="58"/>
       <c r="B77" s="8" t="s">
         <v>54</v>
       </c>
@@ -4845,10 +4949,10 @@
       <c r="D77" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="49" t="s">
+      <c r="E77" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="F77" s="45" t="s">
+      <c r="F77" s="42" t="s">
         <v>5</v>
       </c>
       <c r="G77" s="12" t="s">
@@ -4856,7 +4960,7 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="51"/>
+      <c r="A78" s="58"/>
       <c r="B78" s="8" t="s">
         <v>53</v>
       </c>
@@ -4866,10 +4970,10 @@
       <c r="D78" s="8">
         <v>41.67</v>
       </c>
-      <c r="E78" s="49">
+      <c r="E78" s="46">
         <v>1506.31</v>
       </c>
-      <c r="F78" s="45">
+      <c r="F78" s="42">
         <v>1.6284722222222223</v>
       </c>
       <c r="G78" s="12" t="s">
@@ -4877,19 +4981,20 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A68:A71"/>
     <mergeCell ref="A72:A75"/>
     <mergeCell ref="A76:A78"/>
     <mergeCell ref="O30:P30"/>
-    <mergeCell ref="B1:S1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G60:I60"/>
     <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="O43:P43"/>
+    <mergeCell ref="B1:R1"/>
   </mergeCells>
   <conditionalFormatting sqref="B4:H4 H5:H57">
-    <cfRule type="expression" dxfId="21" priority="45">
+    <cfRule type="expression" dxfId="20" priority="45">
       <formula>$B4 =1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4944,22 +5049,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThanOrEqual">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="8" priority="3">
       <formula>$B4 =1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:I57">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThanOrEqual">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:I57">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$B5 =1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6679,14 +6784,14 @@
       <c r="B2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="44" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44" t="s">
+      <c r="C2" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="44"/>
+      <c r="F2" s="63"/>
       <c r="M2" s="8" t="s">
         <v>21</v>
       </c>
@@ -8386,20 +8491,20 @@
       <c r="C2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="47" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="47" t="s">
         <v>8</v>
       </c>
       <c r="I2" s="19" t="str">
-        <f>CONCATENATE(C2," * x",A2,B2," + ")</f>
+        <f t="shared" ref="I2:I33" si="0">CONCATENATE(C2," * x",A2,B2," + ")</f>
         <v xml:space="preserve">Actual Driving Time * xFromTo + </v>
       </c>
     </row>
@@ -8420,7 +8525,7 @@
         <v>0.63</v>
       </c>
       <c r="F3" s="40">
-        <f>C3*E3</f>
+        <f t="shared" ref="F3:F34" si="1">C3*E3</f>
         <v>134.19</v>
       </c>
       <c r="G3" s="41">
@@ -8428,7 +8533,7 @@
         <v>0.13653846153846153</v>
       </c>
       <c r="I3" t="str">
-        <f>CONCATENATE(C3," * x",A3,B3," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">213 * x12 + </v>
       </c>
     </row>
@@ -8449,15 +8554,15 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F4" s="40">
-        <f>C4*E4</f>
+        <f t="shared" si="1"/>
         <v>108.35000000000001</v>
       </c>
       <c r="G4" s="41">
-        <f t="shared" ref="G4:G56" si="0">(C4/65)/24</f>
+        <f t="shared" ref="G4:G56" si="2">(C4/65)/24</f>
         <v>0.12628205128205128</v>
       </c>
       <c r="I4" t="str">
-        <f>CONCATENATE(C4," * x",A4,B4," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">197 * x13 + </v>
       </c>
     </row>
@@ -8478,15 +8583,15 @@
         <v>0.74</v>
       </c>
       <c r="F5" s="40">
-        <f>C5*E5</f>
+        <f t="shared" si="1"/>
         <v>252.34</v>
       </c>
       <c r="G5" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.21858974358974359</v>
       </c>
       <c r="I5" t="str">
-        <f>CONCATENATE(C5," * x",A5,B5," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">341 * x14 + </v>
       </c>
     </row>
@@ -8507,15 +8612,15 @@
         <v>0.67</v>
       </c>
       <c r="F6" s="40">
-        <f>C6*E6</f>
+        <f t="shared" si="1"/>
         <v>154.10000000000002</v>
       </c>
       <c r="G6" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.14743589743589744</v>
       </c>
       <c r="I6" t="str">
-        <f>CONCATENATE(C6," * x",A6,B6," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">230 * x24 + </v>
       </c>
     </row>
@@ -8536,15 +8641,15 @@
         <v>0.8</v>
       </c>
       <c r="F7" s="40">
-        <f>C7*E7</f>
+        <f t="shared" si="1"/>
         <v>268.8</v>
       </c>
       <c r="G7" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.2153846153846154</v>
       </c>
       <c r="I7" t="str">
-        <f>CONCATENATE(C7," * x",A7,B7," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">336 * x25 + </v>
       </c>
     </row>
@@ -8565,15 +8670,15 @@
         <v>0.69</v>
       </c>
       <c r="F8" s="40">
-        <f>C8*E8</f>
+        <f t="shared" si="1"/>
         <v>206.99999999999997</v>
       </c>
       <c r="G8" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19230769230769229</v>
       </c>
       <c r="I8" t="str">
-        <f>CONCATENATE(C8," * x",A8,B8," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">300 * x34 + </v>
       </c>
     </row>
@@ -8594,15 +8699,15 @@
         <v>0.89</v>
       </c>
       <c r="F9" s="40">
-        <f>C9*E9</f>
+        <f t="shared" si="1"/>
         <v>196.69</v>
       </c>
       <c r="G9" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.14166666666666666</v>
       </c>
       <c r="I9" t="str">
-        <f>CONCATENATE(C9," * x",A9,B9," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">221 * x36 + </v>
       </c>
     </row>
@@ -8623,15 +8728,15 @@
         <v>0.91</v>
       </c>
       <c r="F10" s="40">
-        <f>C10*E10</f>
+        <f t="shared" si="1"/>
         <v>226.59</v>
       </c>
       <c r="G10" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.15961538461538463</v>
       </c>
       <c r="I10" t="str">
-        <f>CONCATENATE(C10," * x",A10,B10," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">249 * x45 + </v>
       </c>
     </row>
@@ -8652,15 +8757,15 @@
         <v>0.93</v>
       </c>
       <c r="F11" s="40">
-        <f>C11*E11</f>
+        <f t="shared" si="1"/>
         <v>294.81</v>
       </c>
       <c r="G11" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.20320512820512823</v>
       </c>
       <c r="I11" t="str">
-        <f>CONCATENATE(C11," * x",A11,B11," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">317 * x46 + </v>
       </c>
     </row>
@@ -8681,15 +8786,15 @@
         <v>0.8</v>
       </c>
       <c r="F12" s="40">
-        <f>C12*E12</f>
+        <f t="shared" si="1"/>
         <v>234.4</v>
       </c>
       <c r="G12" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18782051282051282</v>
       </c>
       <c r="I12" t="str">
-        <f>CONCATENATE(C12," * x",A12,B12," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">293 * x47 + </v>
       </c>
     </row>
@@ -8710,15 +8815,15 @@
         <v>0.73</v>
       </c>
       <c r="F13" s="40">
-        <f>C13*E13</f>
+        <f t="shared" si="1"/>
         <v>315.36</v>
       </c>
       <c r="G13" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.27692307692307694</v>
       </c>
       <c r="I13" t="str">
-        <f>CONCATENATE(C13," * x",A13,B13," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">432 * x57 + </v>
       </c>
     </row>
@@ -8739,15 +8844,15 @@
         <v>0.75</v>
       </c>
       <c r="F14" s="40">
-        <f>C14*E14</f>
+        <f t="shared" si="1"/>
         <v>151.5</v>
       </c>
       <c r="G14" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1294871794871795</v>
       </c>
       <c r="I14" t="str">
-        <f>CONCATENATE(C14," * x",A14,B14," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">202 * x58 + </v>
       </c>
     </row>
@@ -8768,15 +8873,15 @@
         <v>0.91</v>
       </c>
       <c r="F15" s="40">
-        <f>C15*E15</f>
+        <f t="shared" si="1"/>
         <v>362.18</v>
       </c>
       <c r="G15" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.25512820512820511</v>
       </c>
       <c r="I15" t="str">
-        <f>CONCATENATE(C15," * x",A15,B15," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">398 * x67 + </v>
       </c>
     </row>
@@ -8797,15 +8902,15 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="F16" s="40">
-        <f>C16*E16</f>
+        <f t="shared" si="1"/>
         <v>211.7</v>
       </c>
       <c r="G16" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.23397435897435895</v>
       </c>
       <c r="I16" t="str">
-        <f>CONCATENATE(C16," * x",A16,B16," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">365 * x69 + </v>
       </c>
     </row>
@@ -8826,15 +8931,15 @@
         <v>0.6</v>
       </c>
       <c r="F17" s="40">
-        <f>C17*E17</f>
+        <f t="shared" si="1"/>
         <v>207</v>
       </c>
       <c r="G17" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.22115384615384615</v>
       </c>
       <c r="I17" t="str">
-        <f>CONCATENATE(C17," * x",A17,B17," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">345 * x78 + </v>
       </c>
     </row>
@@ -8855,15 +8960,15 @@
         <v>0.61</v>
       </c>
       <c r="F18" s="40">
-        <f>C18*E18</f>
+        <f t="shared" si="1"/>
         <v>93.33</v>
       </c>
       <c r="G18" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.8076923076923075E-2</v>
       </c>
       <c r="I18" t="str">
-        <f>CONCATENATE(C18," * x",A18,B18," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">153 * x79 + </v>
       </c>
     </row>
@@ -8884,15 +8989,15 @@
         <v>0.65</v>
       </c>
       <c r="F19" s="40">
-        <f>C19*E19</f>
+        <f t="shared" si="1"/>
         <v>245.70000000000002</v>
       </c>
       <c r="G19" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.24230769230769231</v>
       </c>
       <c r="I19" t="str">
-        <f>CONCATENATE(C19," * x",A19,B19," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">378 * x710 + </v>
       </c>
     </row>
@@ -8913,15 +9018,15 @@
         <v>0.7</v>
       </c>
       <c r="F20" s="40">
-        <f>C20*E20</f>
+        <f t="shared" si="1"/>
         <v>357.7</v>
       </c>
       <c r="G20" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.32756410256410257</v>
       </c>
       <c r="I20" t="str">
-        <f>CONCATENATE(C20," * x",A20,B20," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">511 * x810 + </v>
       </c>
     </row>
@@ -8942,15 +9047,15 @@
         <v>0.68</v>
       </c>
       <c r="F21" s="40">
-        <f>C21*E21</f>
+        <f t="shared" si="1"/>
         <v>194.48000000000002</v>
       </c>
       <c r="G21" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18333333333333335</v>
       </c>
       <c r="I21" t="str">
-        <f>CONCATENATE(C21," * x",A21,B21," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">286 * x811 + </v>
       </c>
     </row>
@@ -8971,15 +9076,15 @@
         <v>0.76</v>
       </c>
       <c r="F22" s="40">
-        <f>C22*E22</f>
+        <f t="shared" si="1"/>
         <v>316.92</v>
       </c>
       <c r="G22" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.2673076923076923</v>
       </c>
       <c r="I22" t="str">
-        <f>CONCATENATE(C22," * x",A22,B22," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">417 * x910 + </v>
       </c>
     </row>
@@ -9000,15 +9105,15 @@
         <v>0.74</v>
       </c>
       <c r="F23" s="40">
-        <f>C23*E23</f>
+        <f t="shared" si="1"/>
         <v>334.48</v>
       </c>
       <c r="G23" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28974358974358977</v>
       </c>
       <c r="I23" t="str">
-        <f>CONCATENATE(C23," * x",A23,B23," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">452 * x912 + </v>
       </c>
     </row>
@@ -9029,15 +9134,15 @@
         <v>0.93</v>
       </c>
       <c r="F24" s="40">
-        <f>C24*E24</f>
+        <f t="shared" si="1"/>
         <v>429.66</v>
       </c>
       <c r="G24" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.29615384615384616</v>
       </c>
       <c r="I24" t="str">
-        <f>CONCATENATE(C24," * x",A24,B24," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">462 * x1011 + </v>
       </c>
     </row>
@@ -9058,15 +9163,15 @@
         <v>0.89</v>
       </c>
       <c r="F25" s="40">
-        <f>C25*E25</f>
+        <f t="shared" si="1"/>
         <v>178</v>
       </c>
       <c r="G25" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.12820512820512822</v>
       </c>
       <c r="I25" t="str">
-        <f>CONCATENATE(C25," * x",A25,B25," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">200 * x1012 + </v>
       </c>
     </row>
@@ -9087,15 +9192,15 @@
         <v>0.96</v>
       </c>
       <c r="F26" s="40">
-        <f>C26*E26</f>
+        <f t="shared" si="1"/>
         <v>292.8</v>
       </c>
       <c r="G26" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19551282051282051</v>
       </c>
       <c r="I26" t="str">
-        <f>CONCATENATE(C26," * x",A26,B26," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">305 * x1013 + </v>
       </c>
     </row>
@@ -9116,15 +9221,15 @@
         <v>0.78</v>
       </c>
       <c r="F27" s="40">
-        <f>C27*E27</f>
+        <f t="shared" si="1"/>
         <v>477.36</v>
       </c>
       <c r="G27" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.3923076923076923</v>
       </c>
       <c r="I27" t="str">
-        <f>CONCATENATE(C27," * x",A27,B27," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">612 * x1113 + </v>
       </c>
     </row>
@@ -9145,15 +9250,15 @@
         <v>0.75</v>
       </c>
       <c r="F28" s="40">
-        <f>C28*E28</f>
+        <f t="shared" si="1"/>
         <v>202.5</v>
       </c>
       <c r="G28" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1730769230769231</v>
       </c>
       <c r="I28" t="str">
-        <f>CONCATENATE(C28," * x",A28,B28," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">270 * x1114 + </v>
       </c>
     </row>
@@ -9174,15 +9279,15 @@
         <v>0.99</v>
       </c>
       <c r="F29" s="40">
-        <f>C29*E29</f>
+        <f t="shared" si="1"/>
         <v>311.85000000000002</v>
       </c>
       <c r="G29" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.2019230769230769</v>
       </c>
       <c r="I29" t="str">
-        <f>CONCATENATE(C29," * x",A29,B29," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">315 * x1213 + </v>
       </c>
     </row>
@@ -9203,15 +9308,15 @@
         <v>0.66</v>
       </c>
       <c r="F30" s="40">
-        <f>C30*E30</f>
+        <f t="shared" si="1"/>
         <v>275.88</v>
       </c>
       <c r="G30" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.26794871794871794</v>
       </c>
       <c r="I30" t="str">
-        <f>CONCATENATE(C30," * x",A30,B30," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">418 * x1215 + </v>
       </c>
     </row>
@@ -9232,15 +9337,15 @@
         <v>0.97</v>
       </c>
       <c r="F31" s="40">
-        <f>C31*E31</f>
+        <f t="shared" si="1"/>
         <v>532.53</v>
       </c>
       <c r="G31" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.35192307692307695</v>
       </c>
       <c r="I31" t="str">
-        <f>CONCATENATE(C31," * x",A31,B31," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">549 * x1314 + </v>
       </c>
     </row>
@@ -9261,15 +9366,15 @@
         <v>0.72</v>
       </c>
       <c r="F32" s="40">
-        <f>C32*E32</f>
+        <f t="shared" si="1"/>
         <v>186.48</v>
       </c>
       <c r="G32" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.16602564102564102</v>
       </c>
       <c r="I32" t="str">
-        <f>CONCATENATE(C32," * x",A32,B32," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">259 * x1315 + </v>
       </c>
     </row>
@@ -9290,15 +9395,15 @@
         <v>0.95</v>
       </c>
       <c r="F33" s="40">
-        <f>C33*E33</f>
+        <f t="shared" si="1"/>
         <v>251.75</v>
       </c>
       <c r="G33" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.16987179487179485</v>
       </c>
       <c r="I33" t="str">
-        <f>CONCATENATE(C33," * x",A33,B33," + ")</f>
+        <f t="shared" si="0"/>
         <v xml:space="preserve">265 * x1316 + </v>
       </c>
     </row>
@@ -9319,15 +9424,15 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="F34" s="40">
-        <f>C34*E34</f>
+        <f t="shared" si="1"/>
         <v>344.40000000000003</v>
       </c>
       <c r="G34" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.39423076923076922</v>
       </c>
       <c r="I34" t="str">
-        <f>CONCATENATE(C34," * x",A34,B34," + ")</f>
+        <f t="shared" ref="I34:I56" si="3">CONCATENATE(C34," * x",A34,B34," + ")</f>
         <v xml:space="preserve">615 * x1416 + </v>
       </c>
     </row>
@@ -9348,15 +9453,15 @@
         <v>0.62</v>
       </c>
       <c r="F35" s="40">
-        <f>C35*E35</f>
+        <f t="shared" ref="F35:F66" si="4">C35*E35</f>
         <v>155.62</v>
       </c>
       <c r="G35" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.16089743589743591</v>
       </c>
       <c r="I35" t="str">
-        <f>CONCATENATE(C35," * x",A35,B35," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">251 * x1417 + </v>
       </c>
     </row>
@@ -9377,15 +9482,15 @@
         <v>0.79</v>
       </c>
       <c r="F36" s="40">
-        <f>C36*E36</f>
+        <f t="shared" si="4"/>
         <v>233.84</v>
       </c>
       <c r="G36" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18974358974358974</v>
       </c>
       <c r="I36" t="str">
-        <f>CONCATENATE(C36," * x",A36,B36," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">296 * x1516 + </v>
       </c>
     </row>
@@ -9406,15 +9511,15 @@
         <v>0.88</v>
       </c>
       <c r="F37" s="40">
-        <f>C37*E37</f>
+        <f t="shared" si="4"/>
         <v>299.2</v>
       </c>
       <c r="G37" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.21794871794871795</v>
       </c>
       <c r="I37" t="str">
-        <f>CONCATENATE(C37," * x",A37,B37," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">340 * x1518 + </v>
       </c>
     </row>
@@ -9435,15 +9540,15 @@
         <v>0.93</v>
       </c>
       <c r="F38" s="40">
-        <f>C38*E38</f>
+        <f t="shared" si="4"/>
         <v>465</v>
       </c>
       <c r="G38" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.32051282051282054</v>
       </c>
       <c r="I38" t="str">
-        <f>CONCATENATE(C38," * x",A38,B38," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">500 * x1617 + </v>
       </c>
     </row>
@@ -9464,15 +9569,15 @@
         <v>0.74</v>
       </c>
       <c r="F39" s="40">
-        <f>C39*E39</f>
+        <f t="shared" si="4"/>
         <v>256.77999999999997</v>
       </c>
       <c r="G39" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.22243589743589742</v>
       </c>
       <c r="I39" t="str">
-        <f>CONCATENATE(C39," * x",A39,B39," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">347 * x1618 + </v>
       </c>
     </row>
@@ -9493,15 +9598,15 @@
         <v>0.84</v>
       </c>
       <c r="F40" s="40">
-        <f>C40*E40</f>
+        <f t="shared" si="4"/>
         <v>204.12</v>
       </c>
       <c r="G40" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.15576923076923077</v>
       </c>
       <c r="I40" t="str">
-        <f>CONCATENATE(C40," * x",A40,B40," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">243 * x1619 + </v>
       </c>
     </row>
@@ -9522,15 +9627,15 @@
         <v>0.6</v>
       </c>
       <c r="F41" s="40">
-        <f>C41*E41</f>
+        <f t="shared" si="4"/>
         <v>366</v>
       </c>
       <c r="G41" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.39102564102564102</v>
       </c>
       <c r="I41" t="str">
-        <f>CONCATENATE(C41," * x",A41,B41," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">610 * x1719 + </v>
       </c>
     </row>
@@ -9551,15 +9656,15 @@
         <v>0.7</v>
       </c>
       <c r="F42" s="40">
-        <f>C42*E42</f>
+        <f t="shared" si="4"/>
         <v>123.89999999999999</v>
       </c>
       <c r="G42" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11346153846153846</v>
       </c>
       <c r="I42" t="str">
-        <f>CONCATENATE(C42," * x",A42,B42," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">177 * x1720 + </v>
       </c>
     </row>
@@ -9580,15 +9685,15 @@
         <v>0.71</v>
       </c>
       <c r="F43" s="40">
-        <f>C43*E43</f>
+        <f t="shared" si="4"/>
         <v>191.7</v>
       </c>
       <c r="G43" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1730769230769231</v>
       </c>
       <c r="I43" t="str">
-        <f>CONCATENATE(C43," * x",A43,B43," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">270 * x1819 + </v>
       </c>
     </row>
@@ -9609,15 +9714,15 @@
         <v>0.85</v>
       </c>
       <c r="F44" s="40">
-        <f>C44*E44</f>
+        <f t="shared" si="4"/>
         <v>243.1</v>
       </c>
       <c r="G44" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18333333333333335</v>
       </c>
       <c r="I44" t="str">
-        <f>CONCATENATE(C44," * x",A44,B44," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">286 * x1821 + </v>
       </c>
     </row>
@@ -9638,15 +9743,15 @@
         <v>0.99</v>
       </c>
       <c r="F45" s="40">
-        <f>C45*E45</f>
+        <f t="shared" si="4"/>
         <v>464.31</v>
       </c>
       <c r="G45" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.30064102564102563</v>
       </c>
       <c r="I45" t="str">
-        <f>CONCATENATE(C45," * x",A45,B45," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">469 * x1920 + </v>
       </c>
     </row>
@@ -9667,15 +9772,15 @@
         <v>0.72</v>
       </c>
       <c r="F46" s="40">
-        <f>C46*E46</f>
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
       <c r="G46" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.16025641025641027</v>
       </c>
       <c r="I46" t="str">
-        <f>CONCATENATE(C46," * x",A46,B46," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">250 * x1921 + </v>
       </c>
     </row>
@@ -9696,15 +9801,15 @@
         <v>0.6</v>
       </c>
       <c r="F47" s="40">
-        <f>C47*E47</f>
+        <f t="shared" si="4"/>
         <v>138.6</v>
       </c>
       <c r="G47" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.14807692307692308</v>
       </c>
       <c r="I47" t="str">
-        <f>CONCATENATE(C47," * x",A47,B47," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">231 * x1922 + </v>
       </c>
     </row>
@@ -9725,15 +9830,15 @@
         <v>0.65</v>
       </c>
       <c r="F48" s="40">
-        <f>C48*E48</f>
+        <f t="shared" si="4"/>
         <v>332.8</v>
       </c>
       <c r="G48" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.3282051282051282</v>
       </c>
       <c r="I48" t="str">
-        <f>CONCATENATE(C48," * x",A48,B48," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">512 * x2022 + </v>
       </c>
     </row>
@@ -9754,15 +9859,15 @@
         <v>0.65</v>
       </c>
       <c r="F49" s="40">
-        <f>C49*E49</f>
+        <f t="shared" si="4"/>
         <v>265.2</v>
       </c>
       <c r="G49" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.26153846153846155</v>
       </c>
       <c r="I49" t="str">
-        <f>CONCATENATE(C49," * x",A49,B49," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">408 * x2023 + </v>
       </c>
     </row>
@@ -9783,15 +9888,15 @@
         <v>0.98</v>
       </c>
       <c r="F50" s="40">
-        <f>C50*E50</f>
+        <f t="shared" si="4"/>
         <v>245</v>
       </c>
       <c r="G50" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.16025641025641027</v>
       </c>
       <c r="I50" t="str">
-        <f>CONCATENATE(C50," * x",A50,B50," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">250 * x2122 + </v>
       </c>
     </row>
@@ -9812,15 +9917,15 @@
         <v>0.82</v>
       </c>
       <c r="F51" s="40">
-        <f>C51*E51</f>
+        <f t="shared" si="4"/>
         <v>166.45999999999998</v>
       </c>
       <c r="G51" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.13012820512820514</v>
       </c>
       <c r="I51" t="str">
-        <f>CONCATENATE(C51," * x",A51,B51," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">203 * x2124 + </v>
       </c>
     </row>
@@ -9841,15 +9946,15 @@
         <v>0.63</v>
       </c>
       <c r="F52" s="40">
-        <f>C52*E52</f>
+        <f t="shared" si="4"/>
         <v>101.43</v>
       </c>
       <c r="G52" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.10320512820512821</v>
       </c>
       <c r="I52" t="str">
-        <f>CONCATENATE(C52," * x",A52,B52," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">161 * x2223 + </v>
       </c>
     </row>
@@ -9870,15 +9975,15 @@
         <v>0.65</v>
       </c>
       <c r="F53" s="40">
-        <f>C53*E53</f>
+        <f t="shared" si="4"/>
         <v>59.15</v>
       </c>
       <c r="G53" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.8333333333333327E-2</v>
       </c>
       <c r="I53" t="str">
-        <f>CONCATENATE(C53," * x",A53,B53," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">91 * x2224 + </v>
       </c>
     </row>
@@ -9899,15 +10004,15 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="F54" s="40">
-        <f>C54*E54</f>
+        <f t="shared" si="4"/>
         <v>96.320000000000007</v>
       </c>
       <c r="G54" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.11025641025641025</v>
       </c>
       <c r="I54" t="str">
-        <f>CONCATENATE(C54," * x",A54,B54," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">172 * x2225 + </v>
       </c>
     </row>
@@ -9928,15 +10033,15 @@
         <v>0.64</v>
       </c>
       <c r="F55" s="40">
-        <f>C55*E55</f>
+        <f t="shared" si="4"/>
         <v>228.48000000000002</v>
       </c>
       <c r="G55" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.22884615384615384</v>
       </c>
       <c r="I55" t="str">
-        <f>CONCATENATE(C55," * x",A55,B55," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">357 * x2325 + </v>
       </c>
     </row>
@@ -9957,46 +10062,46 @@
         <v>0.66</v>
       </c>
       <c r="F56" s="40">
-        <f>C56*E56</f>
+        <f t="shared" si="4"/>
         <v>100.32000000000001</v>
       </c>
       <c r="G56" s="41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>9.7435897435897437E-2</v>
       </c>
       <c r="I56" t="str">
-        <f>CONCATENATE(C56," * x",A56,B56," + ")</f>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">152 * x2425 + </v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="9" priority="6" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThanOrEqual">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:D56">
-    <cfRule type="expression" dxfId="8" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>#REF! =1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D56">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThanOrEqual">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F56">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>#REF! =1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:G56">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>#REF! =1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E56">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>#REF! =1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>